<commit_message>
Starting to Add Debit and Credit Note
</commit_message>
<xml_diff>
--- a/Goval.FacturaDigital.BusinessService/Files/DefaultInvoices/FacturaGovalFormatoOriginal.xlsx
+++ b/Goval.FacturaDigital.BusinessService/Files/DefaultInvoices/FacturaGovalFormatoOriginal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DV\Goval.FacturaDigital.BusinessService\Goval.FacturaDigital.BusinessService\Files\DefaultInvoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA827EB5-B3F5-453B-9C42-7BCDACA182D1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE77A207-7573-4C80-AE46-F94A4993C25C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <definedName name="clientTaxes">Sheet1!$J$36</definedName>
     <definedName name="clientTelephone">Sheet1!$D$8</definedName>
     <definedName name="clientTerm">Sheet1!$L$5</definedName>
+    <definedName name="documentKey">Sheet1!$E$6</definedName>
     <definedName name="productAmount0">Sheet1!$A$14</definedName>
     <definedName name="productAmount1">Sheet1!$A$15</definedName>
     <definedName name="productAmount10">Sheet1!$A$24</definedName>
@@ -156,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -291,6 +292,9 @@
   </si>
   <si>
     <t xml:space="preserve">      Email:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clave Documento: </t>
   </si>
 </sst>
 </file>
@@ -646,7 +650,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -836,7 +840,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -845,49 +862,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -932,22 +916,43 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1321,24 +1326,24 @@
   <dimension ref="A1:V441"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="1" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="9.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="19.44140625" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" style="6" customWidth="1"/>
-    <col min="14" max="15" width="9.109375" style="9"/>
-    <col min="16" max="16" width="15.44140625" style="7" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" style="6" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="9"/>
+    <col min="16" max="16" width="15.42578125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1">
@@ -1393,16 +1398,16 @@
         <v>16</v>
       </c>
       <c r="L3" s="85"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="101"/>
     </row>
     <row r="4" spans="1:22" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="82" t="s">
@@ -1429,10 +1434,10 @@
       </c>
       <c r="B5" s="82"/>
       <c r="C5" s="82"/>
-      <c r="D5" s="125">
+      <c r="D5" s="90">
         <v>302680516</v>
       </c>
-      <c r="E5" s="125"/>
+      <c r="E5" s="90"/>
       <c r="F5" s="84"/>
       <c r="G5" s="82"/>
       <c r="H5" s="82"/>
@@ -1445,7 +1450,9 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:22" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="4"/>
+      <c r="A6" s="127" t="s">
+        <v>45</v>
+      </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1465,7 +1472,7 @@
       </c>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
-      <c r="D7" s="126"/>
+      <c r="D7" s="89"/>
       <c r="E7" s="81"/>
       <c r="F7" s="81"/>
       <c r="G7" s="81"/>
@@ -1550,21 +1557,21 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:22" ht="15" customHeight="1">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="96"/>
+      <c r="B12" s="92"/>
       <c r="C12" s="65"/>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="96"/>
-      <c r="F12" s="94" t="s">
+      <c r="E12" s="92"/>
+      <c r="F12" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="95"/>
-      <c r="H12" s="95"/>
-      <c r="I12" s="96"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="92"/>
       <c r="J12" s="29" t="s">
         <v>10</v>
       </c>
@@ -1577,17 +1584,17 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1">
-      <c r="A13" s="92"/>
-      <c r="B13" s="93"/>
+      <c r="A13" s="115"/>
+      <c r="B13" s="116"/>
       <c r="C13" s="66"/>
       <c r="D13" s="76"/>
       <c r="E13" s="76"/>
-      <c r="F13" s="92" t="s">
+      <c r="F13" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="93"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="116"/>
       <c r="J13" s="27" t="s">
         <v>11</v>
       </c>
@@ -1599,30 +1606,30 @@
       <c r="O13" s="73"/>
     </row>
     <row r="14" spans="1:22" ht="15" customHeight="1">
-      <c r="A14" s="104"/>
-      <c r="B14" s="105"/>
+      <c r="A14" s="125"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="13"/>
-      <c r="D14" s="121"/>
-      <c r="E14" s="122"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="121"/>
-      <c r="H14" s="121"/>
-      <c r="I14" s="122"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="114"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="94"/>
       <c r="J14" s="77"/>
       <c r="K14" s="28"/>
       <c r="L14" s="70"/>
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:22" ht="15" customHeight="1">
-      <c r="A15" s="102"/>
-      <c r="B15" s="103"/>
+      <c r="A15" s="123"/>
+      <c r="B15" s="124"/>
       <c r="C15" s="34"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="91"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="96"/>
       <c r="J15" s="78"/>
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
@@ -1634,12 +1641,12 @@
       <c r="A16" s="24"/>
       <c r="B16" s="25"/>
       <c r="C16" s="34"/>
-      <c r="D16" s="90"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="90"/>
-      <c r="I16" s="91"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="96"/>
       <c r="J16" s="78"/>
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
@@ -1651,12 +1658,12 @@
       <c r="A17" s="24"/>
       <c r="B17" s="25"/>
       <c r="C17" s="34"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="91"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="96"/>
       <c r="J17" s="78"/>
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
@@ -1668,12 +1675,12 @@
       <c r="A18" s="24"/>
       <c r="B18" s="25"/>
       <c r="C18" s="34"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="91"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="96"/>
       <c r="J18" s="78"/>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
@@ -1685,12 +1692,12 @@
       <c r="A19" s="24"/>
       <c r="B19" s="25"/>
       <c r="C19" s="34"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="91"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="96"/>
       <c r="J19" s="78"/>
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
@@ -1702,12 +1709,12 @@
       <c r="A20" s="24"/>
       <c r="B20" s="25"/>
       <c r="C20" s="34"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="91"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="96"/>
       <c r="J20" s="78"/>
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
@@ -1716,15 +1723,15 @@
       <c r="Q20" s="15"/>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1">
-      <c r="A21" s="102"/>
-      <c r="B21" s="103"/>
+      <c r="A21" s="123"/>
+      <c r="B21" s="124"/>
       <c r="C21" s="34"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="90"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="91"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="96"/>
       <c r="J21" s="78"/>
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
@@ -1733,15 +1740,15 @@
       <c r="Q21" s="14"/>
     </row>
     <row r="22" spans="1:17" ht="15" customHeight="1">
-      <c r="A22" s="102"/>
-      <c r="B22" s="103"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="124"/>
       <c r="C22" s="34"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="90"/>
-      <c r="H22" s="90"/>
-      <c r="I22" s="91"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="96"/>
       <c r="J22" s="78"/>
       <c r="K22" s="28"/>
       <c r="L22" s="28"/>
@@ -1753,12 +1760,12 @@
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
       <c r="C23" s="34"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="90"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="91"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="96"/>
       <c r="J23" s="78"/>
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
@@ -1767,15 +1774,15 @@
       <c r="Q23" s="15"/>
     </row>
     <row r="24" spans="1:17" ht="15" customHeight="1">
-      <c r="A24" s="102"/>
-      <c r="B24" s="103"/>
+      <c r="A24" s="123"/>
+      <c r="B24" s="124"/>
       <c r="C24" s="34"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="91"/>
-      <c r="F24" s="89"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="90"/>
-      <c r="I24" s="91"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="96"/>
       <c r="J24" s="78"/>
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
@@ -1784,15 +1791,15 @@
       <c r="Q24" s="15"/>
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1">
-      <c r="A25" s="102"/>
-      <c r="B25" s="103"/>
+      <c r="A25" s="123"/>
+      <c r="B25" s="124"/>
       <c r="C25" s="34"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="90"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="91"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="95"/>
+      <c r="H25" s="95"/>
+      <c r="I25" s="96"/>
       <c r="J25" s="78"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
@@ -1801,15 +1808,15 @@
       <c r="Q25" s="14"/>
     </row>
     <row r="26" spans="1:17" ht="15" customHeight="1">
-      <c r="A26" s="102"/>
-      <c r="B26" s="103"/>
+      <c r="A26" s="123"/>
+      <c r="B26" s="124"/>
       <c r="C26" s="34"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="90"/>
-      <c r="I26" s="91"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="96"/>
       <c r="J26" s="79"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
@@ -1821,12 +1828,12 @@
       <c r="A27" s="24"/>
       <c r="B27" s="25"/>
       <c r="C27" s="34"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="91"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="96"/>
       <c r="J27" s="78"/>
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
@@ -1838,12 +1845,12 @@
       <c r="A28" s="24"/>
       <c r="B28" s="25"/>
       <c r="C28" s="34"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="91"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="91"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="95"/>
+      <c r="I28" s="96"/>
       <c r="J28" s="78"/>
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
@@ -1852,53 +1859,53 @@
       <c r="Q28" s="15"/>
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1">
-      <c r="A29" s="100"/>
-      <c r="B29" s="101"/>
+      <c r="A29" s="121"/>
+      <c r="B29" s="122"/>
       <c r="C29" s="34"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="91"/>
-      <c r="F29" s="108" t="s">
+      <c r="D29" s="95"/>
+      <c r="E29" s="96"/>
+      <c r="F29" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="G29" s="109"/>
-      <c r="H29" s="109"/>
-      <c r="I29" s="110"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="104"/>
       <c r="J29" s="78"/>
       <c r="K29" s="28"/>
       <c r="L29" s="71"/>
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1">
-      <c r="A30" s="100"/>
-      <c r="B30" s="101"/>
+      <c r="A30" s="121"/>
+      <c r="B30" s="122"/>
       <c r="C30" s="34"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="108"/>
-      <c r="G30" s="109"/>
-      <c r="H30" s="109"/>
-      <c r="I30" s="110"/>
+      <c r="D30" s="95"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="104"/>
       <c r="J30" s="78"/>
       <c r="K30" s="28"/>
       <c r="L30" s="71"/>
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1">
-      <c r="A31" s="98"/>
-      <c r="B31" s="99"/>
+      <c r="A31" s="119"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="68"/>
-      <c r="D31" s="123"/>
-      <c r="E31" s="124"/>
-      <c r="F31" s="117"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="119"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="111"/>
+      <c r="G31" s="112"/>
+      <c r="H31" s="112"/>
+      <c r="I31" s="113"/>
       <c r="J31" s="80"/>
       <c r="K31" s="37"/>
       <c r="L31" s="72"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="13.8">
+    <row r="32" spans="1:17" ht="14.25">
       <c r="A32" s="38"/>
       <c r="B32" s="38"/>
       <c r="C32" s="38"/>
@@ -1913,7 +1920,7 @@
       <c r="L32" s="32"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="33" spans="1:17" ht="19.7" customHeight="1">
       <c r="A33" s="38"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -1923,16 +1930,16 @@
       <c r="G33" s="38"/>
       <c r="H33" s="38"/>
       <c r="I33" s="38"/>
-      <c r="J33" s="111" t="s">
+      <c r="J33" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="K33" s="112"/>
+      <c r="K33" s="106"/>
       <c r="L33" s="46"/>
       <c r="M33" s="1"/>
       <c r="P33" s="18"/>
       <c r="Q33" s="17"/>
     </row>
-    <row r="34" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="34" spans="1:17" ht="19.7" customHeight="1">
       <c r="A34" s="38"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -1942,16 +1949,16 @@
       <c r="G34" s="38"/>
       <c r="H34" s="38"/>
       <c r="I34" s="38"/>
-      <c r="J34" s="115" t="s">
+      <c r="J34" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="K34" s="116"/>
+      <c r="K34" s="110"/>
       <c r="L34" s="47"/>
       <c r="M34" s="1"/>
       <c r="P34" s="18"/>
       <c r="Q34" s="17"/>
     </row>
-    <row r="35" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="35" spans="1:17" ht="19.7" customHeight="1">
       <c r="A35" s="88" t="s">
         <v>36</v>
       </c>
@@ -1963,16 +1970,16 @@
       <c r="G35" s="49"/>
       <c r="H35" s="49"/>
       <c r="I35" s="38"/>
-      <c r="J35" s="115" t="s">
+      <c r="J35" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="K35" s="116"/>
+      <c r="K35" s="110"/>
       <c r="L35" s="47"/>
       <c r="M35" s="1"/>
       <c r="P35" s="18"/>
       <c r="Q35" s="17"/>
     </row>
-    <row r="36" spans="1:17" ht="19.2" customHeight="1">
+    <row r="36" spans="1:17" ht="19.149999999999999" customHeight="1">
       <c r="A36" s="69"/>
       <c r="B36" s="50"/>
       <c r="C36" s="50"/>
@@ -1982,16 +1989,16 @@
       <c r="G36" s="50"/>
       <c r="H36" s="50"/>
       <c r="I36" s="50"/>
-      <c r="J36" s="115" t="s">
+      <c r="J36" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="K36" s="116"/>
+      <c r="K36" s="110"/>
       <c r="L36" s="47"/>
       <c r="M36" s="1"/>
       <c r="P36" s="18"/>
       <c r="Q36" s="17"/>
     </row>
-    <row r="37" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="37" spans="1:17" ht="19.7" customHeight="1">
       <c r="A37" s="49"/>
       <c r="B37" s="49"/>
       <c r="C37" s="49"/>
@@ -2001,16 +2008,16 @@
       <c r="G37" s="49"/>
       <c r="H37" s="49"/>
       <c r="I37" s="38"/>
-      <c r="J37" s="113" t="s">
+      <c r="J37" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="K37" s="114"/>
+      <c r="K37" s="108"/>
       <c r="L37" s="48"/>
       <c r="M37" s="1"/>
       <c r="P37" s="18"/>
       <c r="Q37" s="17"/>
     </row>
-    <row r="38" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="38" spans="1:17" ht="19.7" customHeight="1">
       <c r="A38" s="38"/>
       <c r="B38" s="38"/>
       <c r="C38" s="38"/>
@@ -2027,7 +2034,7 @@
       <c r="P38" s="18"/>
       <c r="Q38" s="17"/>
     </row>
-    <row r="39" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="39" spans="1:17" ht="19.7" customHeight="1">
       <c r="A39" s="88" t="s">
         <v>23</v>
       </c>
@@ -2046,7 +2053,7 @@
       <c r="P39" s="18"/>
       <c r="Q39" s="17"/>
     </row>
-    <row r="40" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="40" spans="1:17" ht="19.7" customHeight="1">
       <c r="A40" s="49"/>
       <c r="B40" s="49"/>
       <c r="C40" s="49"/>
@@ -2063,7 +2070,7 @@
       <c r="P40" s="18"/>
       <c r="Q40" s="17"/>
     </row>
-    <row r="41" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="41" spans="1:17" ht="19.7" customHeight="1">
       <c r="A41" s="49" t="s">
         <v>24</v>
       </c>
@@ -2082,7 +2089,7 @@
       <c r="P41" s="18"/>
       <c r="Q41" s="17"/>
     </row>
-    <row r="42" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="42" spans="1:17" ht="19.7" customHeight="1">
       <c r="A42" s="49" t="s">
         <v>14</v>
       </c>
@@ -2101,7 +2108,7 @@
       <c r="P42" s="18"/>
       <c r="Q42" s="17"/>
     </row>
-    <row r="43" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="43" spans="1:17" ht="19.7" customHeight="1">
       <c r="A43" s="49" t="s">
         <v>25</v>
       </c>
@@ -2120,7 +2127,7 @@
       <c r="P43" s="18"/>
       <c r="Q43" s="17"/>
     </row>
-    <row r="44" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="44" spans="1:17" ht="19.7" customHeight="1">
       <c r="A44" s="49"/>
       <c r="B44" s="49"/>
       <c r="C44" s="49"/>
@@ -2137,7 +2144,7 @@
       <c r="P44" s="18"/>
       <c r="Q44" s="17"/>
     </row>
-    <row r="45" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="45" spans="1:17" ht="19.7" customHeight="1">
       <c r="A45" s="49" t="s">
         <v>28</v>
       </c>
@@ -2156,7 +2163,7 @@
       <c r="P45" s="18"/>
       <c r="Q45" s="17"/>
     </row>
-    <row r="46" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="46" spans="1:17" ht="19.7" customHeight="1">
       <c r="A46" s="54" t="s">
         <v>29</v>
       </c>
@@ -2164,10 +2171,10 @@
       <c r="C46" s="55"/>
       <c r="D46" s="55"/>
       <c r="E46" s="55"/>
-      <c r="F46" s="106" t="s">
+      <c r="F46" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="G46" s="106"/>
+      <c r="G46" s="97"/>
       <c r="H46" s="56" t="s">
         <v>34</v>
       </c>
@@ -2179,7 +2186,7 @@
       <c r="P46" s="18"/>
       <c r="Q46" s="17"/>
     </row>
-    <row r="47" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="47" spans="1:17" ht="19.7" customHeight="1">
       <c r="A47" s="54" t="s">
         <v>30</v>
       </c>
@@ -2187,10 +2194,10 @@
       <c r="C47" s="55"/>
       <c r="D47" s="55"/>
       <c r="E47" s="55"/>
-      <c r="F47" s="106" t="s">
+      <c r="F47" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="G47" s="106"/>
+      <c r="G47" s="97"/>
       <c r="H47" s="56" t="s">
         <v>34</v>
       </c>
@@ -2202,7 +2209,7 @@
       <c r="P47" s="18"/>
       <c r="Q47" s="17"/>
     </row>
-    <row r="48" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="48" spans="1:17" ht="19.7" customHeight="1">
       <c r="A48" s="54" t="s">
         <v>31</v>
       </c>
@@ -2210,10 +2217,10 @@
       <c r="C48" s="55"/>
       <c r="D48" s="55"/>
       <c r="E48" s="55"/>
-      <c r="F48" s="106" t="s">
+      <c r="F48" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="G48" s="106"/>
+      <c r="G48" s="97"/>
       <c r="H48" s="56" t="s">
         <v>34</v>
       </c>
@@ -2225,7 +2232,7 @@
       <c r="P48" s="18"/>
       <c r="Q48" s="17"/>
     </row>
-    <row r="49" spans="1:17" ht="19.649999999999999" customHeight="1">
+    <row r="49" spans="1:17" ht="19.7" customHeight="1">
       <c r="A49" s="49"/>
       <c r="B49" s="52"/>
       <c r="C49" s="52"/>
@@ -2299,7 +2306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="15.6">
+    <row r="53" spans="1:17" ht="15">
       <c r="A53" s="58" t="s">
         <v>42</v>
       </c>
@@ -2316,7 +2323,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:17" ht="15.6">
+    <row r="54" spans="1:17" ht="15">
       <c r="A54" s="61"/>
       <c r="B54" s="63"/>
       <c r="C54" s="63"/>
@@ -9287,30 +9294,27 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
     <mergeCell ref="F47:G47"/>
     <mergeCell ref="F48:G48"/>
     <mergeCell ref="M3:V3"/>
@@ -9327,27 +9331,30 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="F20:I20"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>